<commit_message>
Started on Items documentation
</commit_message>
<xml_diff>
--- a/ItemsDoc.xlsx
+++ b/ItemsDoc.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ItemsList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="164">
   <si>
     <t>ActionButton</t>
   </si>
@@ -433,9 +433,6 @@
     <t>Power Meter</t>
   </si>
   <si>
-    <t>Wireless power consumptino meter</t>
-  </si>
-  <si>
     <t>Remote Switch/Dimmer using the FS20 system</t>
   </si>
   <si>
@@ -473,6 +470,42 @@
   </si>
   <si>
     <t>The WEB interface used to configure and use OpenNetHome</t>
+  </si>
+  <si>
+    <t>Wireless power consumption meter</t>
+  </si>
+  <si>
+    <t>PHILIPS Hue</t>
+  </si>
+  <si>
+    <t>Zigbee</t>
+  </si>
+  <si>
+    <t>Connects to the PHILPS Hue bridge device which controls a Hue system</t>
+  </si>
+  <si>
+    <t>RF Bulb</t>
+  </si>
+  <si>
+    <t>PHILPS Hue remote controlled lamp bulb</t>
+  </si>
+  <si>
+    <t>IKEA Trådfri</t>
+  </si>
+  <si>
+    <t>IKEA Trådfri remote controlled lamp bulb with adjustable color temperature</t>
+  </si>
+  <si>
+    <t>IKEA Trådfri remote gateway</t>
+  </si>
+  <si>
+    <t>IKEA Trådfri remote controlled lamp bulb</t>
+  </si>
+  <si>
+    <t>Delay timer with repeating actions</t>
+  </si>
+  <si>
+    <t>Item and firmware to use JeeLink Classic as RF Transmitter for 433MHz remote control</t>
   </si>
 </sst>
 </file>
@@ -1297,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1432,7 +1465,7 @@
         <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>124</v>
@@ -1452,7 +1485,7 @@
         <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>125</v>
@@ -1540,7 +1573,7 @@
         <v>138</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1557,7 +1590,7 @@
         <v>138</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1574,7 +1607,7 @@
         <v>123</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1594,7 +1627,7 @@
         <v>123</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1602,10 +1635,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1616,16 +1649,16 @@
         <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
         <v>115</v>
       </c>
       <c r="E20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1636,10 +1669,10 @@
         <v>110</v>
       </c>
       <c r="C21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1647,13 +1680,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1664,48 +1697,138 @@
         <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
+        <v>154</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" t="s">
+        <v>154</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:6">

</xml_diff>

<commit_message>
Updated Items documentation - now complete!
</commit_message>
<xml_diff>
--- a/ItemsDoc.xlsx
+++ b/ItemsDoc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="262">
   <si>
     <t>ActionButton</t>
   </si>
@@ -250,9 +250,6 @@
     <t>UPMRainfall</t>
   </si>
   <si>
-    <t>UPMSoilMoisture</t>
-  </si>
-  <si>
     <t>UPMThermometer</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
     <t>ZWaveNode</t>
   </si>
   <si>
-    <t>ZWaveNodeExplorer</t>
-  </si>
-  <si>
     <t>ZWaveRemapButton</t>
   </si>
   <si>
@@ -364,9 +358,6 @@
     <t>Sunset Control</t>
   </si>
   <si>
-    <t>Week timer with suppport for sun rise/sun set control</t>
-  </si>
-  <si>
     <t>Add/remove debug logging from Items</t>
   </si>
   <si>
@@ -676,7 +667,139 @@
     <t>Connects to a Telldus TellstickDuo 433MHz remote control</t>
   </si>
   <si>
-    <t>Separate WEB GUI to present thermometer values</t>
+    <t>Separate WEB GUI to present thermometer values and graphs</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Display a tray bar icon for OpenNetHome Server on the desktop</t>
+  </si>
+  <si>
+    <t>Control any function via commands in UDP/IP messages</t>
+  </si>
+  <si>
+    <t>Recieves UDP-Messages</t>
+  </si>
+  <si>
+    <t>UPM</t>
+  </si>
+  <si>
+    <t>Wireless hygrometer using the UPM protocol</t>
+  </si>
+  <si>
+    <t>Wireless rain gauge using the UPM protocol</t>
+  </si>
+  <si>
+    <t>Wireless thermometer using the UPM protocol</t>
+  </si>
+  <si>
+    <t>Wireless wind direction sensor using the UPM protocol</t>
+  </si>
+  <si>
+    <t>Wireless wind speed sensor using the UPM protocol</t>
+  </si>
+  <si>
+    <t>Built in Item that detects devices via the Universal Plug&amp;Play (UPnP) protocol</t>
+  </si>
+  <si>
+    <t>Auto Detect</t>
+  </si>
+  <si>
+    <t>Built in Item that detects devices connected via USB</t>
+  </si>
+  <si>
+    <t>Can log the value of any attribute in another Item and presents graphs of the value</t>
+  </si>
+  <si>
+    <t>Monitors the value of an attribute in an Item and triggers actions based on the value</t>
+  </si>
+  <si>
+    <t>Waveman</t>
+  </si>
+  <si>
+    <t>Control remote switches using Waveman protocol</t>
+  </si>
+  <si>
+    <t>Week timer (Use SunTimer)</t>
+  </si>
+  <si>
+    <t>Week timer with suppport for sun rise/sun set control (Use SunTimer)</t>
+  </si>
+  <si>
+    <t>Belkin Wemo</t>
+  </si>
+  <si>
+    <t>Connects to Belkin Wemo remote controlled light bulbs</t>
+  </si>
+  <si>
+    <t>Belkin Wemo remote controlled switch with power usage sensor</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Belkin Wemo remote controlled light bulb (needs WemoBridge)</t>
+  </si>
+  <si>
+    <t>Belkin Wemo remote controlled switch</t>
+  </si>
+  <si>
+    <t>XMPP</t>
+  </si>
+  <si>
+    <t>JABBER</t>
+  </si>
+  <si>
+    <t>Client for sending and receiving XAMPP (Jabber) messages</t>
+  </si>
+  <si>
+    <t>Zhejiang</t>
+  </si>
+  <si>
+    <t>Control remote switches using Zhejiang protocol</t>
+  </si>
+  <si>
+    <t>Z-Wave</t>
+  </si>
+  <si>
+    <t>Control Z-Wave window blinds</t>
+  </si>
+  <si>
+    <t>Map Z-Wave Central Scene commands to actions on other Items</t>
+  </si>
+  <si>
+    <t>Telnet command prompt for sending and receiving Z-Wave commands</t>
+  </si>
+  <si>
+    <t>Connects to a Z-Wave Controller/USB Dongle</t>
+  </si>
+  <si>
+    <t>Controls a Z-Wave dimmer</t>
+  </si>
+  <si>
+    <t>Remote Dimmers</t>
+  </si>
+  <si>
+    <t>Controls a Z-Wave switch</t>
+  </si>
+  <si>
+    <t>Controls a Z-Wave sensor</t>
+  </si>
+  <si>
+    <t>Represents a general Z-Wave node. Is automatically created when a node is discovered</t>
+  </si>
+  <si>
+    <t>Map Z-Wave commands to actions on other Items</t>
+  </si>
+  <si>
+    <t>Plugins</t>
+  </si>
+  <si>
+    <t>Mac OSX</t>
   </si>
 </sst>
 </file>
@@ -1161,9 +1284,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1501,17 +1625,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="80" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1519,10 +1644,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1530,10 +1655,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>240</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1541,19 +1669,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="D3" t="s">
-        <v>112</v>
-      </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1561,19 +1689,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
         <v>110</v>
       </c>
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
       <c r="E4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1581,13 +1709,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>111</v>
+        <v>204</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1595,13 +1723,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1609,16 +1737,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
         <v>113</v>
       </c>
-      <c r="C7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" t="s">
-        <v>115</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>116</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1626,10 +1754,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1637,19 +1765,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1657,19 +1785,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1677,16 +1805,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1694,19 +1822,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1714,19 +1842,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" t="s">
         <v>124</v>
       </c>
-      <c r="D13" t="s">
-        <v>127</v>
-      </c>
       <c r="E13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1734,19 +1862,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1754,19 +1882,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1774,19 +1902,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1794,16 +1922,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1811,19 +1939,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1831,10 +1959,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1842,19 +1970,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1862,13 +1990,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1876,13 +2004,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1890,19 +2018,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1910,16 +2038,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1927,19 +2055,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" t="s">
         <v>146</v>
       </c>
-      <c r="C25" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="F25" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="E25" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1947,19 +2075,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E26" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1967,16 +2095,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1984,19 +2112,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C28" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" t="s">
-        <v>147</v>
-      </c>
-      <c r="E28" t="s">
-        <v>149</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2004,13 +2132,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2018,16 +2146,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2035,13 +2163,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2049,16 +2177,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2066,16 +2194,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2083,13 +2211,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C34" t="s">
-        <v>162</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2097,13 +2225,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+      <c r="D35" t="s">
+        <v>240</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2111,13 +2242,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2125,13 +2256,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2139,13 +2270,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2153,13 +2284,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>126</v>
+      </c>
+      <c r="D39" t="s">
+        <v>241</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2167,16 +2301,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2184,19 +2318,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" t="s">
+        <v>207</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C41" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" t="s">
-        <v>210</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2204,19 +2338,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2224,19 +2358,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D43" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2244,19 +2378,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2264,19 +2398,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2284,19 +2418,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2304,19 +2438,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2324,19 +2458,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
+        <v>177</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2344,19 +2478,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
+        <v>255</v>
       </c>
       <c r="D49" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E49" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2364,19 +2498,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E50" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2384,19 +2518,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E51" t="s">
+        <v>177</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2404,19 +2538,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E52" t="s">
+        <v>177</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2424,19 +2558,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E53" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2444,19 +2578,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D54" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E54" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2464,19 +2598,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E55" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2484,19 +2618,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C56" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D56" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E56" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2504,19 +2638,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D57" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E57" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2524,13 +2658,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2538,19 +2672,19 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E59" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2558,19 +2692,19 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D60" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E60" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2578,19 +2712,19 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C61" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" t="s">
         <v>110</v>
       </c>
-      <c r="D61" t="s">
-        <v>112</v>
-      </c>
       <c r="E61" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2598,19 +2732,19 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D62" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E62" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2618,19 +2752,19 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C63" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D63" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E63" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2638,19 +2772,19 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C64" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D64" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E64" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2658,13 +2792,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2672,10 +2806,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2683,16 +2817,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67" t="s">
         <v>113</v>
       </c>
-      <c r="C67" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67" t="s">
-        <v>115</v>
-      </c>
       <c r="F67" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2700,16 +2834,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D68" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2717,16 +2851,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C69" t="s">
+        <v>207</v>
+      </c>
+      <c r="D69" t="s">
+        <v>132</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D69" t="s">
-        <v>135</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2734,13 +2868,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2748,16 +2882,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2765,19 +2899,19 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C72" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D72" t="s">
         <v>71</v>
       </c>
       <c r="E72" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2785,173 +2919,503 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>218</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="B75" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" t="s">
+        <v>207</v>
+      </c>
+      <c r="D75" t="s">
+        <v>132</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" t="s">
+        <v>207</v>
+      </c>
+      <c r="D76" t="s">
+        <v>132</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="B77" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" t="s">
+        <v>121</v>
+      </c>
+      <c r="D77" t="s">
+        <v>122</v>
+      </c>
+      <c r="E77" t="s">
+        <v>222</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="B78" t="s">
+        <v>107</v>
+      </c>
+      <c r="C78" t="s">
+        <v>121</v>
+      </c>
+      <c r="D78" t="s">
+        <v>124</v>
+      </c>
+      <c r="E78" t="s">
+        <v>222</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="B79" t="s">
+        <v>107</v>
+      </c>
+      <c r="C79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D79" t="s">
+        <v>126</v>
+      </c>
+      <c r="E79" t="s">
+        <v>222</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80" t="s">
+        <v>121</v>
+      </c>
+      <c r="D80" t="s">
+        <v>190</v>
+      </c>
+      <c r="E80" t="s">
+        <v>222</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81" t="s">
+        <v>107</v>
+      </c>
+      <c r="C81" t="s">
+        <v>121</v>
+      </c>
+      <c r="D81" t="s">
+        <v>190</v>
+      </c>
+      <c r="E81" t="s">
+        <v>222</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" t="s">
+        <v>229</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83" t="s">
+        <v>229</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" t="s">
+        <v>137</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85" t="s">
+        <v>105</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" t="s">
+        <v>115</v>
+      </c>
+      <c r="D86" t="s">
+        <v>110</v>
+      </c>
+      <c r="E86" t="s">
+        <v>233</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87" t="s">
+        <v>105</v>
+      </c>
+      <c r="C87" t="s">
+        <v>111</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88" t="s">
+        <v>237</v>
+      </c>
+      <c r="C88" t="s">
+        <v>110</v>
+      </c>
+      <c r="D88" t="s">
+        <v>144</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89" t="s">
+        <v>237</v>
+      </c>
+      <c r="C89" t="s">
+        <v>110</v>
+      </c>
+      <c r="D89" t="s">
+        <v>121</v>
+      </c>
+      <c r="E89" t="s">
+        <v>115</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90" t="s">
+        <v>237</v>
+      </c>
+      <c r="C90" t="s">
+        <v>110</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91" t="s">
+        <v>237</v>
+      </c>
+      <c r="C91" t="s">
+        <v>110</v>
+      </c>
+      <c r="D91" t="s">
+        <v>115</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92" t="s">
+        <v>244</v>
+      </c>
+      <c r="C92" t="s">
+        <v>245</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" t="s">
+        <v>115</v>
+      </c>
+      <c r="D93" t="s">
+        <v>110</v>
+      </c>
+      <c r="E93" t="s">
+        <v>247</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94" t="s">
+        <v>249</v>
+      </c>
+      <c r="C94" t="s">
+        <v>200</v>
+      </c>
+      <c r="D94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95" t="s">
+        <v>249</v>
+      </c>
+      <c r="C95" t="s">
+        <v>105</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96" t="s">
+        <v>249</v>
+      </c>
+      <c r="C96" t="s">
+        <v>105</v>
+      </c>
+      <c r="D96" t="s">
+        <v>207</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97" t="s">
+        <v>249</v>
+      </c>
+      <c r="C97" t="s">
+        <v>110</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98" t="s">
+        <v>249</v>
+      </c>
+      <c r="C98" t="s">
+        <v>255</v>
+      </c>
+      <c r="D98" t="s">
+        <v>110</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99" t="s">
+        <v>249</v>
+      </c>
+      <c r="C99" t="s">
+        <v>115</v>
+      </c>
+      <c r="D99" t="s">
+        <v>110</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100" t="s">
+        <v>249</v>
+      </c>
+      <c r="C100" t="s">
+        <v>121</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101" t="s">
+        <v>249</v>
+      </c>
+      <c r="C101" t="s">
+        <v>121</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102" t="s">
+        <v>249</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="1" t="s">
-        <v>104</v>
+      <c r="B103" t="s">
+        <v>249</v>
+      </c>
+      <c r="C103" t="s">
+        <v>105</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="B104" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="B105" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added skeleton to document generator
</commit_message>
<xml_diff>
--- a/ItemsDoc.xlsx
+++ b/ItemsDoc.xlsx
@@ -7873,7 +7873,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:A315"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8230,8 +8230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D315"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41:D42"/>
+    <sheetView topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8253,8 +8253,8 @@
         <v>212</v>
       </c>
       <c r="D1" t="str">
-        <f>"&lt;strong class=""card""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A1 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A1 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C1</f>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=AudioProtocolParser" target="_blank" rel="noopener noreferrer"&gt;AudioProtocolParser&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Decodes RF/IR messages for DIY RF recievers. Lot of built in decoders</v>
+        <f>"&lt;strong class=""item""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A1 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A1 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C1</f>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=AudioProtocolParser" target="_blank" rel="noopener noreferrer"&gt;AudioProtocolParser&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Decodes RF/IR messages for DIY RF recievers. Lot of built in decoders</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8268,8 +8268,8 @@
         <v>211</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D65" si="0">"&lt;strong class=""card""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A2 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A2 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C2</f>
-        <v xml:space="preserve">&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=AudioProtocolTransmitter" target="_blank" rel="noopener noreferrer"&gt;AudioProtocolTransmitter&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Encodes RF/IR messages for DIY RF transmitters. Lot of built in encoders </v>
+        <f t="shared" ref="D2:D65" si="0">"&lt;strong class=""item""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A2 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A2 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C2</f>
+        <v xml:space="preserve">&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=AudioProtocolTransmitter" target="_blank" rel="noopener noreferrer"&gt;AudioProtocolTransmitter&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Encodes RF/IR messages for DIY RF transmitters. Lot of built in encoders </v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8284,7 +8284,7 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=CULTransceiver" target="_blank" rel="noopener noreferrer"&gt;CULTransceiver&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Item and firmware to use CUL HW as RF Transmitter for 433MHz remote control</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=CULTransceiver" target="_blank" rel="noopener noreferrer"&gt;CULTransceiver&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Item and firmware to use CUL HW as RF Transmitter for 433MHz remote control</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8299,7 +8299,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DeltronicLamp" target="_blank" rel="noopener noreferrer"&gt;DeltronicLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Deltronic-protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DeltronicLamp" target="_blank" rel="noopener noreferrer"&gt;DeltronicLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Deltronic-protocol</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8314,7 +8314,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DeltronicRemapButton" target="_blank" rel="noopener noreferrer"&gt;DeltronicRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Deltronic protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DeltronicRemapButton" target="_blank" rel="noopener noreferrer"&gt;DeltronicRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Deltronic protocol</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8329,7 +8329,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FineOffsetHygrometer" target="_blank" rel="noopener noreferrer"&gt;FineOffsetHygrometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless hygrometer using the FineOffset protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FineOffsetHygrometer" target="_blank" rel="noopener noreferrer"&gt;FineOffsetHygrometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless hygrometer using the FineOffset protocol</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -8344,7 +8344,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FineOffsetRainGauge" target="_blank" rel="noopener noreferrer"&gt;FineOffsetRainGauge&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless rain gauge using the FineOffset protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FineOffsetRainGauge" target="_blank" rel="noopener noreferrer"&gt;FineOffsetRainGauge&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless rain gauge using the FineOffset protocol</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -8359,7 +8359,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FineOffsetThermometer" target="_blank" rel="noopener noreferrer"&gt;FineOffsetThermometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless thermometer using the FineOffset protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FineOffsetThermometer" target="_blank" rel="noopener noreferrer"&gt;FineOffsetThermometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless thermometer using the FineOffset protocol</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8374,7 +8374,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FooGadgetLegacy" target="_blank" rel="noopener noreferrer"&gt;FooGadgetLegacy&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless power consumption meter</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FooGadgetLegacy" target="_blank" rel="noopener noreferrer"&gt;FooGadgetLegacy&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless power consumption meter</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -8389,7 +8389,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FooGadgetPulse" target="_blank" rel="noopener noreferrer"&gt;FooGadgetPulse&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless power consumption meter</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FooGadgetPulse" target="_blank" rel="noopener noreferrer"&gt;FooGadgetPulse&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless power consumption meter</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -8404,7 +8404,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=GenericProntoCommander" target="_blank" rel="noopener noreferrer"&gt;GenericProntoCommander&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Send recorded RF/IR commands using the Pronto format</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=GenericProntoCommander" target="_blank" rel="noopener noreferrer"&gt;GenericProntoCommander&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Send recorded RF/IR commands using the Pronto format</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -8419,7 +8419,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=JeeLink" target="_blank" rel="noopener noreferrer"&gt;JeeLink&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Item and firmware to use JeeLink Classic as RF Transmitter for 433MHz remote control</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=JeeLink" target="_blank" rel="noopener noreferrer"&gt;JeeLink&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Item and firmware to use JeeLink Classic as RF Transmitter for 433MHz remote control</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -8434,7 +8434,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLamp" target="_blank" rel="noopener noreferrer"&gt;NexaLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Nexa-protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLamp" target="_blank" rel="noopener noreferrer"&gt;NexaLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Nexa-protocol</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -8449,7 +8449,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCAdvancedRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCAdvancedRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCAdvancedRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCAdvancedRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -8464,7 +8464,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCDimmer" target="_blank" rel="noopener noreferrer"&gt;NexaLCDimmer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote dimmers using Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCDimmer" target="_blank" rel="noopener noreferrer"&gt;NexaLCDimmer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote dimmers using Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -8479,7 +8479,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCLamp" target="_blank" rel="noopener noreferrer"&gt;NexaLCLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCLamp" target="_blank" rel="noopener noreferrer"&gt;NexaLCLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -8509,7 +8509,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton4" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton4&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton4" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton4&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -8524,7 +8524,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa protocol</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -8539,7 +8539,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaSmokeDetector" target="_blank" rel="noopener noreferrer"&gt;NexaSmokeDetector&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions from a smoke detector using the Nexa protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaSmokeDetector" target="_blank" rel="noopener noreferrer"&gt;NexaSmokeDetector&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions from a smoke detector using the Nexa protocol</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -8554,7 +8554,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=OregonHygrometer" target="_blank" rel="noopener noreferrer"&gt;OregonHygrometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless hygrometer using the Oregon Scientific protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=OregonHygrometer" target="_blank" rel="noopener noreferrer"&gt;OregonHygrometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless hygrometer using the Oregon Scientific protocol</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -8569,7 +8569,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=OregonThermometer" target="_blank" rel="noopener noreferrer"&gt;OregonThermometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless thermometer using the Oregon Scientific protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=OregonThermometer" target="_blank" rel="noopener noreferrer"&gt;OregonThermometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless thermometer using the Oregon Scientific protocol</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -8584,7 +8584,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=OregonWind" target="_blank" rel="noopener noreferrer"&gt;OregonWind&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless wind gauge using the Oregon Scientific protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=OregonWind" target="_blank" rel="noopener noreferrer"&gt;OregonWind&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless wind gauge using the Oregon Scientific protocol</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -8599,7 +8599,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ProntoDevice" target="_blank" rel="noopener noreferrer"&gt;ProntoDevice&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Device controlled by sending recorded RF/IR commands using the Pronto format</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ProntoDevice" target="_blank" rel="noopener noreferrer"&gt;ProntoDevice&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Device controlled by sending recorded RF/IR commands using the Pronto format</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -8614,7 +8614,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ProntoLamp" target="_blank" rel="noopener noreferrer"&gt;ProntoLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Lamp controlled by sending recorded RF/IR commands using the Pronto format</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ProntoLamp" target="_blank" rel="noopener noreferrer"&gt;ProntoLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Lamp controlled by sending recorded RF/IR commands using the Pronto format</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -8629,7 +8629,7 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RFBitBangerTransmitter" target="_blank" rel="noopener noreferrer"&gt;RFBitBangerTransmitter&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Encodes RF/IR messages for DIY RF transmitters via RFBitBanger for RaspberryPi</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RFBitBangerTransmitter" target="_blank" rel="noopener noreferrer"&gt;RFBitBangerTransmitter&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Encodes RF/IR messages for DIY RF transmitters via RFBitBanger for RaspberryPi</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -8644,7 +8644,7 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RisingSunLamp" target="_blank" rel="noopener noreferrer"&gt;RisingSunLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using RisingSun protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RisingSunLamp" target="_blank" rel="noopener noreferrer"&gt;RisingSunLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using RisingSun protocol</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -8659,7 +8659,7 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RollerTrolBlind" target="_blank" rel="noopener noreferrer"&gt;RollerTrolBlind&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Controls RollerTroll window blinds</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RollerTrolBlind" target="_blank" rel="noopener noreferrer"&gt;RollerTrolBlind&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Controls RollerTroll window blinds</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -8674,7 +8674,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RollerTrolBlindGSeries" target="_blank" rel="noopener noreferrer"&gt;RollerTrolBlindGSeries&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Controls RollerTroll window blinds</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=RollerTrolBlindGSeries" target="_blank" rel="noopener noreferrer"&gt;RollerTrolBlindGSeries&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Controls RollerTroll window blinds</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -8689,7 +8689,7 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=Tellstick" target="_blank" rel="noopener noreferrer"&gt;Tellstick&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Connects to a Telldus TellstickDuo 433MHz remote control</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=Tellstick" target="_blank" rel="noopener noreferrer"&gt;Tellstick&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Connects to a Telldus TellstickDuo 433MHz remote control</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -8704,7 +8704,7 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMHygrometer" target="_blank" rel="noopener noreferrer"&gt;UPMHygrometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless hygrometer using the UPM protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMHygrometer" target="_blank" rel="noopener noreferrer"&gt;UPMHygrometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless hygrometer using the UPM protocol</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -8719,7 +8719,7 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMRainfall" target="_blank" rel="noopener noreferrer"&gt;UPMRainfall&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless rain gauge using the UPM protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMRainfall" target="_blank" rel="noopener noreferrer"&gt;UPMRainfall&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless rain gauge using the UPM protocol</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -8733,8 +8733,8 @@
         <v>225</v>
       </c>
       <c r="D33" t="str">
-        <f>"&lt;strong class=""card""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A33 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A33 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C33</f>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMThermometer" target="_blank" rel="noopener noreferrer"&gt;UPMThermometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless thermometer using the UPM protocol</v>
+        <f t="shared" si="0"/>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMThermometer" target="_blank" rel="noopener noreferrer"&gt;UPMThermometer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless thermometer using the UPM protocol</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -8749,7 +8749,7 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMWindDirection" target="_blank" rel="noopener noreferrer"&gt;UPMWindDirection&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless wind direction sensor using the UPM protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMWindDirection" target="_blank" rel="noopener noreferrer"&gt;UPMWindDirection&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless wind direction sensor using the UPM protocol</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMWindSpeed" target="_blank" rel="noopener noreferrer"&gt;UPMWindSpeed&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless wind speed sensor using the UPM protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPMWindSpeed" target="_blank" rel="noopener noreferrer"&gt;UPMWindSpeed&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Wireless wind speed sensor using the UPM protocol</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -8779,7 +8779,7 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WavemanLamp" target="_blank" rel="noopener noreferrer"&gt;WavemanLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Waveman protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WavemanLamp" target="_blank" rel="noopener noreferrer"&gt;WavemanLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Waveman protocol</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -8794,7 +8794,7 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZhejiangLamp" target="_blank" rel="noopener noreferrer"&gt;ZhejiangLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Zhejiang protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZhejiangLamp" target="_blank" rel="noopener noreferrer"&gt;ZhejiangLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control remote switches using Zhejiang protocol</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -8808,8 +8808,8 @@
         <v>120</v>
       </c>
       <c r="D38" t="str">
-        <f>"&lt;strong class=""card""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A38 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A38 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C38</f>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FHZ1000PcPort" target="_blank" rel="noopener noreferrer"&gt;FHZ1000PcPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Connect to RF Transmitter from the FS20 remote control system</v>
+        <f t="shared" si="0"/>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FHZ1000PcPort" target="_blank" rel="noopener noreferrer"&gt;FHZ1000PcPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Connect to RF Transmitter from the FS20 remote control system</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -8824,7 +8824,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FS20Lamp" target="_blank" rel="noopener noreferrer"&gt;FS20Lamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Remote Switch/Dimmer using the FS20 system</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FS20Lamp" target="_blank" rel="noopener noreferrer"&gt;FS20Lamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Remote Switch/Dimmer using the FS20 system</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -8839,7 +8839,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FS20RemapButton" target="_blank" rel="noopener noreferrer"&gt;FS20RemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the FS20</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FS20RemapButton" target="_blank" rel="noopener noreferrer"&gt;FS20RemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the FS20</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -8854,7 +8854,7 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPnPScanner" target="_blank" rel="noopener noreferrer"&gt;UPnPScanner&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Built in Item that detects devices via the Universal Plug&amp;Play (UPnP) protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UPnPScanner" target="_blank" rel="noopener noreferrer"&gt;UPnPScanner&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Built in Item that detects devices via the Universal Plug&amp;Play (UPnP) protocol</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -8869,7 +8869,7 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UsbScanner" target="_blank" rel="noopener noreferrer"&gt;UsbScanner&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Built in Item that detects devices connected via USB</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UsbScanner" target="_blank" rel="noopener noreferrer"&gt;UsbScanner&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Built in Item that detects devices connected via USB</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -8884,7 +8884,7 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ArpScanner" target="_blank" rel="noopener noreferrer"&gt;ArpScanner&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Scans for connected network devices (Linux only)</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ArpScanner" target="_blank" rel="noopener noreferrer"&gt;ArpScanner&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Scans for connected network devices (Linux only)</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -8899,7 +8899,7 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DayLiteTimer" target="_blank" rel="noopener noreferrer"&gt;DayLiteTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Week timer with suppport for sun rise/sun set control (Use SunTimer)</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DayLiteTimer" target="_blank" rel="noopener noreferrer"&gt;DayLiteTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Week timer with suppport for sun rise/sun set control (Use SunTimer)</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -8914,7 +8914,7 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DeltronicRemapButton" target="_blank" rel="noopener noreferrer"&gt;DeltronicRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Deltronic protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=DeltronicRemapButton" target="_blank" rel="noopener noreferrer"&gt;DeltronicRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Deltronic protocol</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -8929,7 +8929,7 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FS20RemapButton" target="_blank" rel="noopener noreferrer"&gt;FS20RemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the FS20</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=FS20RemapButton" target="_blank" rel="noopener noreferrer"&gt;FS20RemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the FS20</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -8944,7 +8944,7 @@
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=IntervalTimer" target="_blank" rel="noopener noreferrer"&gt;IntervalTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Delay timer with repeating actions</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=IntervalTimer" target="_blank" rel="noopener noreferrer"&gt;IntervalTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Delay timer with repeating actions</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -8959,7 +8959,7 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=LampGroup" target="_blank" rel="noopener noreferrer"&gt;LampGroup&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Group multiple lamps together so they can be handled together as one lamp</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=LampGroup" target="_blank" rel="noopener noreferrer"&gt;LampGroup&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Group multiple lamps together so they can be handled together as one lamp</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -8974,7 +8974,7 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=LampRepeater" target="_blank" rel="noopener noreferrer"&gt;LampRepeater&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Repeats signals to remote controlled lamps over unreliable RF communication</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=LampRepeater" target="_blank" rel="noopener noreferrer"&gt;LampRepeater&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Repeats signals to remote controlled lamps over unreliable RF communication</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -8989,7 +8989,7 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MacDevice" target="_blank" rel="noopener noreferrer"&gt;MacDevice&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions when a device appears/disappears in the network</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MacDevice" target="_blank" rel="noopener noreferrer"&gt;MacDevice&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions when a device appears/disappears in the network</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -9004,7 +9004,7 @@
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MacDeviceGroup" target="_blank" rel="noopener noreferrer"&gt;MacDeviceGroup&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions when a group of devices appears/disappears in the network</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MacDeviceGroup" target="_blank" rel="noopener noreferrer"&gt;MacDeviceGroup&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions when a group of devices appears/disappears in the network</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -9019,7 +9019,7 @@
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MqttRemapButton" target="_blank" rel="noopener noreferrer"&gt;MqttRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions in Items on receiving MQTT events</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MqttRemapButton" target="_blank" rel="noopener noreferrer"&gt;MqttRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions in Items on receiving MQTT events</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -9034,7 +9034,7 @@
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MqttValueLogger" target="_blank" rel="noopener noreferrer"&gt;MqttValueLogger&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Exposes the value of any attribute in any Item as MQTT events</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=MqttValueLogger" target="_blank" rel="noopener noreferrer"&gt;MqttValueLogger&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Exposes the value of any attribute in any Item as MQTT events</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -9049,7 +9049,7 @@
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCAdvancedRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCAdvancedRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCAdvancedRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCAdvancedRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -9064,7 +9064,7 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -9079,7 +9079,7 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton4" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton4&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaLCRemapButton4" target="_blank" rel="noopener noreferrer"&gt;NexaLCRemapButton4&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa Learning Code protocol</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -9094,7 +9094,7 @@
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaRemapButton" target="_blank" rel="noopener noreferrer"&gt;NexaRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions by a remote control using the Nexa protocol</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -9109,7 +9109,7 @@
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaSmokeDetector" target="_blank" rel="noopener noreferrer"&gt;NexaSmokeDetector&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions from a smoke detector using the Nexa protocol</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=NexaSmokeDetector" target="_blank" rel="noopener noreferrer"&gt;NexaSmokeDetector&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger actions from a smoke detector using the Nexa protocol</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -9124,7 +9124,7 @@
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=Scene" target="_blank" rel="noopener noreferrer"&gt;Scene&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger a number of actions simultainuasly or in a row</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=Scene" target="_blank" rel="noopener noreferrer"&gt;Scene&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Trigger a number of actions simultainuasly or in a row</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -9139,7 +9139,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=SunTimer" target="_blank" rel="noopener noreferrer"&gt;SunTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Week timer with suppport for sun rise/sun set control, variables and random times</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=SunTimer" target="_blank" rel="noopener noreferrer"&gt;SunTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Week timer with suppport for sun rise/sun set control, variables and random times</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -9154,7 +9154,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=TCPCommandPort" target="_blank" rel="noopener noreferrer"&gt;TCPCommandPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control any function via commands on a TCP/IP connection</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=TCPCommandPort" target="_blank" rel="noopener noreferrer"&gt;TCPCommandPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control any function via commands on a TCP/IP connection</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -9169,7 +9169,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=TCPListener" target="_blank" rel="noopener noreferrer"&gt;TCPListener&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Recieves TCP-Messages</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=TCPListener" target="_blank" rel="noopener noreferrer"&gt;TCPListener&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Recieves TCP-Messages</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -9184,7 +9184,7 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UDPCommandPort" target="_blank" rel="noopener noreferrer"&gt;UDPCommandPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control any function via commands in UDP/IP messages</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UDPCommandPort" target="_blank" rel="noopener noreferrer"&gt;UDPCommandPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Control any function via commands in UDP/IP messages</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -9199,7 +9199,7 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UDPListener" target="_blank" rel="noopener noreferrer"&gt;UDPListener&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Recieves UDP-Messages</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=UDPListener" target="_blank" rel="noopener noreferrer"&gt;UDPListener&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Recieves UDP-Messages</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -9214,7 +9214,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ValueLogger" target="_blank" rel="noopener noreferrer"&gt;ValueLogger&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Can log the value of any attribute in another Item and presents graphs of the value</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ValueLogger" target="_blank" rel="noopener noreferrer"&gt;ValueLogger&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Can log the value of any attribute in another Item and presents graphs of the value</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -9228,8 +9228,8 @@
         <v>232</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D74" si="1">"&lt;strong class=""card""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A66 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A66 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C66</f>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ValueTrigger" target="_blank" rel="noopener noreferrer"&gt;ValueTrigger&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Monitors the value of an attribute in an Item and triggers actions based on the value</v>
+        <f t="shared" ref="D66:D74" si="1">"&lt;strong class=""item""&gt;&lt;a href=""http://wiki.nethome.nu/doku.php?id=" &amp; A66 &amp; """ target=""_blank"" rel=""noopener noreferrer""&gt;" &amp; A66 &amp; "&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;" &amp; C66</f>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ValueTrigger" target="_blank" rel="noopener noreferrer"&gt;ValueTrigger&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Monitors the value of an attribute in an Item and triggers actions based on the value</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -9244,7 +9244,7 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WeekTimer" target="_blank" rel="noopener noreferrer"&gt;WeekTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Week timer (Use SunTimer)</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WeekTimer" target="_blank" rel="noopener noreferrer"&gt;WeekTimer&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Week timer (Use SunTimer)</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -9259,7 +9259,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZWaveCentralSceneRemapButton" target="_blank" rel="noopener noreferrer"&gt;ZWaveCentralSceneRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Map Z-Wave Central Scene commands to actions on other Items</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZWaveCentralSceneRemapButton" target="_blank" rel="noopener noreferrer"&gt;ZWaveCentralSceneRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Map Z-Wave Central Scene commands to actions on other Items</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -9274,7 +9274,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZWaveCommandPort" target="_blank" rel="noopener noreferrer"&gt;ZWaveCommandPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Telnet command prompt for sending and receiving Z-Wave commands</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZWaveCommandPort" target="_blank" rel="noopener noreferrer"&gt;ZWaveCommandPort&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Telnet command prompt for sending and receiving Z-Wave commands</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -9289,7 +9289,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZWaveRemapButton" target="_blank" rel="noopener noreferrer"&gt;ZWaveRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Map Z-Wave commands to actions on other Items</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=ZWaveRemapButton" target="_blank" rel="noopener noreferrer"&gt;ZWaveRemapButton&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Map Z-Wave commands to actions on other Items</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -9304,7 +9304,7 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoBridge" target="_blank" rel="noopener noreferrer"&gt;WemoBridge&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Connects to Belkin Wemo remote controlled light bulbs</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoBridge" target="_blank" rel="noopener noreferrer"&gt;WemoBridge&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Connects to Belkin Wemo remote controlled light bulbs</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -9319,7 +9319,7 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoInsightSwitch" target="_blank" rel="noopener noreferrer"&gt;WemoInsightSwitch&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Belkin Wemo remote controlled switch with power usage sensor</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoInsightSwitch" target="_blank" rel="noopener noreferrer"&gt;WemoInsightSwitch&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Belkin Wemo remote controlled switch with power usage sensor</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -9334,7 +9334,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoLamp" target="_blank" rel="noopener noreferrer"&gt;WemoLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Belkin Wemo remote controlled light bulb (needs WemoBridge)</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoLamp" target="_blank" rel="noopener noreferrer"&gt;WemoLamp&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Belkin Wemo remote controlled light bulb (needs WemoBridge)</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -9349,7 +9349,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;strong class="card"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoSwitch" target="_blank" rel="noopener noreferrer"&gt;WemoSwitch&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Belkin Wemo remote controlled switch</v>
+        <v>&lt;strong class="item"&gt;&lt;a href="http://wiki.nethome.nu/doku.php?id=WemoSwitch" target="_blank" rel="noopener noreferrer"&gt;WemoSwitch&lt;/a&gt;&lt;/strong&gt;&amp;nbsp;Belkin Wemo remote controlled switch</v>
       </c>
     </row>
     <row r="75" spans="1:4">

</xml_diff>